<commit_message>
add Procedure IG:Operation and RT
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Condition-profile.xlsx
+++ b/docs/StructureDefinition-Condition-profile.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-07T11:52:30+08:00</t>
+    <t>2022-08-27T12:17:33+08:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example of a profile of Condition(CISCTCAE)</t>
+    <t>Example of a profile of Condition(CISCTCAE)副作用併發症記錄表</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>